<commit_message>
add: Add function of custom key update: Update document
</commit_message>
<xml_diff>
--- a/doc/ATCFS Specifications.xlsx
+++ b/doc/ATCFS Specifications.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$330</definedName>
-    <definedName name="subject" localSheetId="0">Sheet1!$C$291</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$343</definedName>
+    <definedName name="subject" localSheetId="0">Sheet1!$C$292</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="536">
   <si>
     <t>Map</t>
     <phoneticPr fontId="2"/>
@@ -4005,16 +4005,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>2行目以降は、1列目に列車速度[km/h]を昇順で記述してください。値の間隔は一定である必要はありません。</t>
-    <rPh sb="1" eb="3">
-      <t>ギョウメ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>イコウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>ただし、定義できる特性曲線の本数はノッチ1段あたり1本です。</t>
     <rPh sb="4" eb="6">
       <t>テイギ</t>
@@ -4066,6 +4056,207 @@
     </rPh>
     <rPh sb="66" eb="68">
       <t>ダンスウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2行目以降は、1列目に列車速度[km/h]を整数値で、かつ昇順で記述してください。値の間隔は一定である必要はありません。</t>
+    <rPh sb="1" eb="3">
+      <t>ギョウメ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>セイスウ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ats271</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>使用禁止</t>
+    <rPh sb="0" eb="2">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キンシ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>OpenBVE版</t>
+    <rPh sb="7" eb="8">
+      <t>バン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>atcfs_openbve.cfg (For OpenBVE)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SwitchN</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Init</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>カスタムスイッチの状態量の最小値  (デフォルト値=0)</t>
+    <rPh sb="9" eb="11">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>リョウ</t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t>サイショウチ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>カスタムスイッチの状態量の最大値  (デフォルト値=1)</t>
+    <rPh sb="13" eb="16">
+      <t>サイダイチ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>カスタムスイッチの状態量の初期値  (デフォルト値=0)</t>
+    <rPh sb="13" eb="16">
+      <t>ショキチ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Step</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>カスタムスイッチの状態量の単位変化量  (デフォルト値=1)</t>
+    <rPh sb="9" eb="11">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>リョウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>タンイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>リョウ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Loop</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>カスタムスイッチの状態量をループさせるか(0: 無効, 1: 有効)  (デフォルト値=0)</t>
+    <rPh sb="24" eb="26">
+      <t>ムコウ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Key0</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>カスタムスイッチのキー割り当て(右回し)  (デフォルト値なし)</t>
+    <rPh sb="11" eb="12">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>マワ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Key1</t>
+  </si>
+  <si>
+    <t>カスタムスイッチのキー割り当て(左回し)  (デフォルト値なし)</t>
+    <rPh sb="11" eb="12">
+      <t>ワ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>マワ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>(N=0～9)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>カスタムスイッチのパネルインデックスおよびサウンドインデックス (指定可能な値: 0～270)</t>
+    <rPh sb="33" eb="35">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>アタイ</t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -4475,7 +4666,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4719,6 +4910,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4730,33 +4954,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5062,10 +5259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E329"/>
+  <dimension ref="A1:E342"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A311" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B327" sqref="B327"/>
+      <selection activeCell="E336" sqref="E336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -5641,7 +5838,7 @@
       <c r="D52" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="E52" s="82" t="s">
+      <c r="E52" s="93" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5652,14 +5849,14 @@
       </c>
       <c r="C53" s="31"/>
       <c r="D53" s="11"/>
-      <c r="E53" s="81"/>
+      <c r="E53" s="92"/>
     </row>
     <row r="54" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3"/>
       <c r="B54" s="31"/>
       <c r="C54" s="31"/>
       <c r="D54" s="11"/>
-      <c r="E54" s="81" t="s">
+      <c r="E54" s="92" t="s">
         <v>326</v>
       </c>
     </row>
@@ -5668,7 +5865,7 @@
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
       <c r="D55" s="11"/>
-      <c r="E55" s="81"/>
+      <c r="E55" s="92"/>
     </row>
     <row r="56" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="3"/>
@@ -5704,7 +5901,7 @@
       <c r="D59" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="E59" s="82" t="s">
+      <c r="E59" s="93" t="s">
         <v>328</v>
       </c>
     </row>
@@ -5715,7 +5912,7 @@
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="11"/>
-      <c r="E60" s="81"/>
+      <c r="E60" s="92"/>
     </row>
     <row r="61" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
@@ -5753,7 +5950,7 @@
       <c r="D64" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="E64" s="82" t="s">
+      <c r="E64" s="93" t="s">
         <v>331</v>
       </c>
     </row>
@@ -5766,7 +5963,7 @@
       <c r="D65" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="E65" s="81"/>
+      <c r="E65" s="92"/>
     </row>
     <row r="66" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3"/>
@@ -5820,7 +6017,7 @@
       <c r="D71" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="E71" s="82" t="s">
+      <c r="E71" s="93" t="s">
         <v>336</v>
       </c>
     </row>
@@ -5833,7 +6030,7 @@
       <c r="D72" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E72" s="81"/>
+      <c r="E72" s="92"/>
     </row>
     <row r="73" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="3"/>
@@ -5891,7 +6088,7 @@
       <c r="D78" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="E78" s="82" t="s">
+      <c r="E78" s="93" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5904,7 +6101,7 @@
       <c r="D79" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="E79" s="81"/>
+      <c r="E79" s="92"/>
     </row>
     <row r="80" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="3"/>
@@ -5924,7 +6121,7 @@
       <c r="D81" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="E81" s="81" t="s">
+      <c r="E81" s="92" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5935,7 +6132,7 @@
       </c>
       <c r="C82" s="31"/>
       <c r="D82" s="11"/>
-      <c r="E82" s="81"/>
+      <c r="E82" s="92"/>
     </row>
     <row r="83" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="3"/>
@@ -5973,7 +6170,7 @@
       <c r="D86" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E86" s="82" t="s">
+      <c r="E86" s="93" t="s">
         <v>229</v>
       </c>
     </row>
@@ -5986,7 +6183,7 @@
       <c r="D87" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="E87" s="81"/>
+      <c r="E87" s="92"/>
     </row>
     <row r="88" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="3"/>
@@ -6459,7 +6656,7 @@
       <c r="D132" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="E132" s="83" t="s">
+      <c r="E132" s="94" t="s">
         <v>404</v>
       </c>
     </row>
@@ -6468,7 +6665,7 @@
       <c r="B133" s="31"/>
       <c r="C133" s="56"/>
       <c r="D133" s="14"/>
-      <c r="E133" s="84"/>
+      <c r="E133" s="95"/>
     </row>
     <row r="134" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="3"/>
@@ -8413,7 +8610,7 @@
     </row>
     <row r="287" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A287" s="3"/>
-      <c r="B287" s="30"/>
+      <c r="B287" s="24"/>
       <c r="C287" s="35" t="s">
         <v>138</v>
       </c>
@@ -8424,456 +8621,586 @@
         <v>177</v>
       </c>
     </row>
-    <row r="288" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A288" s="3"/>
-      <c r="B288" s="6"/>
-      <c r="C288" s="6"/>
-      <c r="D288" s="6"/>
-      <c r="E288" s="6"/>
+      <c r="B288" s="20" t="s">
+        <v>516</v>
+      </c>
+      <c r="C288" s="35" t="s">
+        <v>514</v>
+      </c>
+      <c r="D288" s="65"/>
+      <c r="E288" s="65" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="289" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3"/>
-      <c r="B289" s="68" t="s">
+      <c r="B289" s="6"/>
+      <c r="C289" s="6"/>
+      <c r="D289" s="6"/>
+      <c r="E289" s="6"/>
+    </row>
+    <row r="290" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A290" s="3"/>
+      <c r="B290" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C289" s="64" t="s">
+      <c r="C290" s="64" t="s">
         <v>415</v>
       </c>
-      <c r="D289" s="54"/>
-      <c r="E289" s="3"/>
-    </row>
-    <row r="290" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A290" s="3"/>
-      <c r="B290" s="3"/>
-      <c r="C290" s="3"/>
-      <c r="D290" s="3"/>
+      <c r="D290" s="54"/>
       <c r="E290" s="3"/>
     </row>
     <row r="291" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A291" s="3"/>
-      <c r="B291" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="C291" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D291" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E291" s="9" t="s">
-        <v>354</v>
-      </c>
+      <c r="B291" s="3"/>
+      <c r="C291" s="3"/>
+      <c r="D291" s="3"/>
+      <c r="E291" s="3"/>
     </row>
     <row r="292" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A292" s="3"/>
-      <c r="B292" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C292" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="D292" s="67" t="s">
-        <v>180</v>
-      </c>
-      <c r="E292" s="65" t="s">
-        <v>305</v>
+      <c r="B292" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C292" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D292" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E292" s="9" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="293" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A293" s="3"/>
-      <c r="B293" s="24"/>
-      <c r="C293" s="69" t="s">
-        <v>182</v>
-      </c>
-      <c r="D293" s="58" t="s">
+      <c r="B293" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C293" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="D293" s="67" t="s">
         <v>180</v>
       </c>
-      <c r="E293" s="67" t="s">
-        <v>487</v>
+      <c r="E293" s="65" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="294" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A294" s="3"/>
-      <c r="B294" s="11"/>
-      <c r="C294" s="25" t="s">
-        <v>68</v>
+      <c r="B294" s="24"/>
+      <c r="C294" s="69" t="s">
+        <v>182</v>
       </c>
       <c r="D294" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E294" s="9" t="s">
-        <v>387</v>
+      <c r="E294" s="67" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A295" s="3"/>
       <c r="B295" s="11"/>
       <c r="C295" s="25" t="s">
-        <v>183</v>
+        <v>68</v>
       </c>
       <c r="D295" s="58" t="s">
         <v>180</v>
       </c>
       <c r="E295" s="9" t="s">
-        <v>474</v>
+        <v>387</v>
       </c>
     </row>
     <row r="296" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A296" s="3"/>
       <c r="B296" s="11"/>
       <c r="C296" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D296" s="58" t="s">
         <v>180</v>
       </c>
       <c r="E296" s="9" t="s">
-        <v>416</v>
+        <v>474</v>
       </c>
     </row>
     <row r="297" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A297" s="3"/>
       <c r="B297" s="11"/>
       <c r="C297" s="25" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D297" s="58" t="s">
         <v>180</v>
       </c>
       <c r="E297" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="298" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A298" s="3"/>
       <c r="B298" s="11"/>
-      <c r="C298" s="70" t="s">
-        <v>212</v>
-      </c>
-      <c r="D298" s="67" t="s">
-        <v>213</v>
-      </c>
-      <c r="E298" s="65" t="s">
-        <v>306</v>
+      <c r="C298" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D298" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="E298" s="9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="299" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A299" s="3"/>
-      <c r="B299" s="24"/>
+      <c r="B299" s="11"/>
       <c r="C299" s="70" t="s">
-        <v>195</v>
-      </c>
-      <c r="D299" s="58" t="s">
-        <v>180</v>
+        <v>212</v>
+      </c>
+      <c r="D299" s="67" t="s">
+        <v>213</v>
       </c>
       <c r="E299" s="65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="300" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A300" s="3"/>
       <c r="B300" s="24"/>
-      <c r="C300" s="69" t="s">
-        <v>196</v>
+      <c r="C300" s="70" t="s">
+        <v>195</v>
       </c>
       <c r="D300" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E300" s="67" t="s">
-        <v>308</v>
+      <c r="E300" s="65" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="301" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A301" s="3"/>
       <c r="B301" s="24"/>
-      <c r="C301" s="70" t="s">
-        <v>476</v>
-      </c>
-      <c r="D301" s="67" t="s">
+      <c r="C301" s="69" t="s">
+        <v>196</v>
+      </c>
+      <c r="D301" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="E301" s="65" t="s">
-        <v>475</v>
+      <c r="E301" s="67" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="302" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A302" s="3"/>
       <c r="B302" s="24"/>
       <c r="C302" s="70" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D302" s="67" t="s">
         <v>180</v>
       </c>
       <c r="E302" s="65" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="303" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A303" s="3"/>
       <c r="B303" s="24"/>
       <c r="C303" s="70" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="D303" s="67" t="s">
         <v>180</v>
       </c>
       <c r="E303" s="65" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="304" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A304" s="3"/>
-      <c r="B304" s="30"/>
+      <c r="B304" s="24"/>
       <c r="C304" s="70" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D304" s="67" t="s">
         <v>180</v>
       </c>
       <c r="E304" s="65" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A305" s="3"/>
+      <c r="B305" s="30"/>
+      <c r="C305" s="70" t="s">
+        <v>484</v>
+      </c>
+      <c r="D305" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E305" s="65" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="305" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="3"/>
-      <c r="B305" s="3"/>
-      <c r="C305" s="3"/>
-      <c r="D305" s="3"/>
-      <c r="E305" s="3"/>
     </row>
     <row r="306" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A306" s="3"/>
-      <c r="B306" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C306" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="B306" s="3"/>
+      <c r="C306" s="3"/>
       <c r="D306" s="3"/>
       <c r="E306" s="3"/>
     </row>
-    <row r="307" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A307" s="3"/>
-      <c r="B307" s="3"/>
-      <c r="C307" s="3"/>
+      <c r="B307" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C307" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="D307" s="3"/>
       <c r="E307" s="3"/>
     </row>
     <row r="308" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A308" s="3"/>
-      <c r="B308" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="C308" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D308" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="E308" s="9" t="s">
-        <v>48</v>
-      </c>
+      <c r="B308" s="3"/>
+      <c r="C308" s="3"/>
+      <c r="D308" s="3"/>
+      <c r="E308" s="3"/>
     </row>
     <row r="309" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A309" s="3"/>
-      <c r="B309" s="19" t="s">
-        <v>55</v>
+      <c r="B309" s="20" t="s">
+        <v>210</v>
       </c>
       <c r="C309" s="20" t="s">
-        <v>185</v>
+        <v>47</v>
       </c>
       <c r="D309" s="20" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E309" s="9" t="s">
-        <v>388</v>
+        <v>48</v>
       </c>
     </row>
     <row r="310" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A310" s="3"/>
-      <c r="B310" s="24"/>
-      <c r="C310" s="35" t="s">
-        <v>214</v>
-      </c>
-      <c r="D310" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="E310" s="65" t="s">
-        <v>309</v>
+      <c r="B310" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C310" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D310" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="E310" s="9" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="311" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A311" s="3"/>
       <c r="B311" s="24"/>
       <c r="C311" s="35" t="s">
-        <v>467</v>
+        <v>214</v>
       </c>
       <c r="D311" s="35" t="s">
-        <v>468</v>
+        <v>215</v>
       </c>
       <c r="E311" s="65" t="s">
-        <v>469</v>
+        <v>309</v>
       </c>
     </row>
     <row r="312" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A312" s="3"/>
       <c r="B312" s="24"/>
       <c r="C312" s="35" t="s">
-        <v>481</v>
-      </c>
-      <c r="D312" s="65" t="s">
-        <v>480</v>
+        <v>467</v>
+      </c>
+      <c r="D312" s="35" t="s">
+        <v>468</v>
       </c>
       <c r="E312" s="65" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
     </row>
     <row r="313" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A313" s="3"/>
-      <c r="B313" s="11"/>
+      <c r="B313" s="24"/>
       <c r="C313" s="35" t="s">
-        <v>188</v>
+        <v>481</v>
       </c>
       <c r="D313" s="65" t="s">
-        <v>310</v>
+        <v>480</v>
       </c>
       <c r="E313" s="65" t="s">
-        <v>189</v>
+        <v>482</v>
       </c>
     </row>
     <row r="314" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A314" s="3"/>
       <c r="B314" s="11"/>
       <c r="C314" s="35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D314" s="65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E314" s="65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="315" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A315" s="3"/>
-      <c r="B315" s="14"/>
+      <c r="B315" s="11"/>
       <c r="C315" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="D315" s="65" t="s">
+        <v>311</v>
+      </c>
+      <c r="E315" s="65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A316" s="3"/>
+      <c r="B316" s="14"/>
+      <c r="C316" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="D315" s="65" t="s">
+      <c r="D316" s="65" t="s">
         <v>312</v>
       </c>
-      <c r="E315" s="65" t="s">
+      <c r="E316" s="65" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="316" spans="1:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="317" spans="1:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B317" s="68" t="s">
+    <row r="317" spans="1:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="318" spans="1:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B318" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C317" s="64" t="s">
+      <c r="C318" s="64" t="s">
         <v>501</v>
       </c>
-      <c r="D317" s="54"/>
-      <c r="E317" s="3"/>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B318" s="3"/>
-      <c r="C318" s="3"/>
-      <c r="D318" s="3"/>
+      <c r="D318" s="54"/>
       <c r="E318" s="3"/>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B319" s="20" t="s">
+      <c r="B319" s="3"/>
+      <c r="C319" s="3"/>
+      <c r="D319" s="3"/>
+      <c r="E319" s="3"/>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B320" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="C319" s="19" t="s">
+      <c r="C320" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="D319" s="9" t="s">
+      <c r="D320" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="E319" s="9" t="s">
+      <c r="E320" s="9" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B320" s="19" t="s">
+    <row r="321" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B321" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C320" s="20" t="s">
+      <c r="C321" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="D320" s="79" t="s">
+      <c r="D321" s="79" t="s">
+        <v>510</v>
+      </c>
+      <c r="E321" s="9" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="322" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B322" s="80"/>
+      <c r="C322" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="D322" s="79" t="s">
+        <v>503</v>
+      </c>
+      <c r="E322" s="9" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="323" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="324" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B324" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C324" s="64" t="s">
+        <v>507</v>
+      </c>
+      <c r="D324" s="54"/>
+    </row>
+    <row r="326" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B326" s="81" t="s">
+        <v>508</v>
+      </c>
+      <c r="C326" s="82"/>
+      <c r="D326" s="82"/>
+      <c r="E326" s="83"/>
+    </row>
+    <row r="327" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B327" s="81" t="s">
+        <v>512</v>
+      </c>
+      <c r="C327" s="82"/>
+      <c r="D327" s="82"/>
+      <c r="E327" s="83"/>
+    </row>
+    <row r="328" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B328" s="84" t="s">
+        <v>513</v>
+      </c>
+      <c r="C328" s="85"/>
+      <c r="D328" s="85"/>
+      <c r="E328" s="86"/>
+    </row>
+    <row r="329" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B329" s="84" t="s">
         <v>511</v>
       </c>
-      <c r="E320" s="9" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="321" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B321" s="80"/>
-      <c r="C321" s="20" t="s">
-        <v>505</v>
-      </c>
-      <c r="D321" s="79" t="s">
-        <v>503</v>
-      </c>
-      <c r="E321" s="9" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="322" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="323" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B323" s="68" t="s">
+      <c r="C329" s="85"/>
+      <c r="D329" s="85"/>
+      <c r="E329" s="86"/>
+    </row>
+    <row r="330" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B330" s="87" t="s">
+        <v>509</v>
+      </c>
+      <c r="C330" s="88"/>
+      <c r="D330" s="88"/>
+      <c r="E330" s="89"/>
+    </row>
+    <row r="331" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="332" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B332" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C323" s="64" t="s">
-        <v>507</v>
-      </c>
-      <c r="D323" s="54"/>
-    </row>
-    <row r="325" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B325" s="85" t="s">
-        <v>508</v>
-      </c>
-      <c r="C325" s="86"/>
-      <c r="D325" s="86"/>
-      <c r="E325" s="87"/>
-    </row>
-    <row r="326" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B326" s="85" t="s">
-        <v>513</v>
-      </c>
-      <c r="C326" s="86"/>
-      <c r="D326" s="86"/>
-      <c r="E326" s="87"/>
-    </row>
-    <row r="327" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B327" s="88" t="s">
-        <v>509</v>
-      </c>
-      <c r="C327" s="89"/>
-      <c r="D327" s="89"/>
-      <c r="E327" s="90"/>
-    </row>
-    <row r="328" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B328" s="88" t="s">
-        <v>512</v>
-      </c>
-      <c r="C328" s="89"/>
-      <c r="D328" s="89"/>
-      <c r="E328" s="90"/>
-    </row>
-    <row r="329" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B329" s="91" t="s">
-        <v>510</v>
-      </c>
-      <c r="C329" s="92"/>
-      <c r="D329" s="92"/>
-      <c r="E329" s="93"/>
+      <c r="C332" s="64" t="s">
+        <v>517</v>
+      </c>
+      <c r="D332" s="54"/>
+      <c r="E332" s="3"/>
+    </row>
+    <row r="333" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B333" s="3"/>
+      <c r="C333" s="3"/>
+      <c r="D333" s="3"/>
+      <c r="E333" s="3"/>
+    </row>
+    <row r="334" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B334" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C334" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="D334" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="E334" s="9" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="335" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B335" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C335" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="D335" s="91" t="s">
+        <v>519</v>
+      </c>
+      <c r="E335" s="9" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="336" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B336" s="31"/>
+      <c r="C336" s="24" t="s">
+        <v>534</v>
+      </c>
+      <c r="D336" s="91" t="s">
+        <v>520</v>
+      </c>
+      <c r="E336" s="9" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="337" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B337" s="31"/>
+      <c r="C337" s="24"/>
+      <c r="D337" s="91" t="s">
+        <v>521</v>
+      </c>
+      <c r="E337" s="9" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="338" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B338" s="31"/>
+      <c r="C338" s="24"/>
+      <c r="D338" s="91" t="s">
+        <v>522</v>
+      </c>
+      <c r="E338" s="9" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="339" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B339" s="31"/>
+      <c r="C339" s="24"/>
+      <c r="D339" s="91" t="s">
+        <v>526</v>
+      </c>
+      <c r="E339" s="9" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="340" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B340" s="31"/>
+      <c r="C340" s="24"/>
+      <c r="D340" s="91" t="s">
+        <v>528</v>
+      </c>
+      <c r="E340" s="9" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="341" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B341" s="31"/>
+      <c r="C341" s="24"/>
+      <c r="D341" s="91" t="s">
+        <v>530</v>
+      </c>
+      <c r="E341" s="9" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="342" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B342" s="90"/>
+      <c r="C342" s="30"/>
+      <c r="D342" s="91" t="s">
+        <v>532</v>
+      </c>
+      <c r="E342" s="9" t="s">
+        <v>533</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -8899,7 +9226,7 @@
     <brk id="157" max="16383" man="1"/>
     <brk id="213" max="4" man="1"/>
     <brk id="259" max="4" man="1"/>
-    <brk id="288" max="16383" man="1"/>
+    <brk id="289" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>